<commit_message>
added plugin to pom:surefire and maven compiler.Created few more testng.xml files for data provider, grouping etc.
</commit_message>
<xml_diff>
--- a/VRadAutomationFramework/src/test/resources/data/VRad_Automation_Data.xlsx
+++ b/VRadAutomationFramework/src/test/resources/data/VRad_Automation_Data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ashwini.g\eclipse-workspace\VRadAutomationFramework\src\test\resources\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ashwini.g\git\VRadAutomation\VRadAutomationFramework\src\test\resources\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D9EE560-8993-4518-918A-B1DE971F5EA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EE689A5-0EA6-4214-B2DF-C0E95F34A7FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -504,15 +504,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18" customWidth="1"/>
-    <col min="2" max="2" width="31.77734375" customWidth="1"/>
-    <col min="3" max="3" width="14.21875" customWidth="1"/>
+    <col min="1" max="1" width="18" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="31.77734375" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="14.21875" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.3">
@@ -607,8 +607,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.77734375" customWidth="1"/>
-    <col min="2" max="2" width="14.33203125" customWidth="1"/>
+    <col min="1" max="1" width="18.77734375" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="14.33203125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
@@ -628,15 +628,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61EA455B-2D2A-421D-9AC3-E9AFD0B1211F}">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.77734375" customWidth="1"/>
-    <col min="2" max="2" width="11" customWidth="1"/>
-    <col min="3" max="4" width="14" customWidth="1"/>
+    <col min="1" max="1" width="12.77734375" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="11" customWidth="1" collapsed="1"/>
+    <col min="3" max="4" width="14" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
@@ -724,8 +724,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.88671875" customWidth="1"/>
-    <col min="2" max="2" width="39" style="5" customWidth="1"/>
+    <col min="1" max="1" width="23.88671875" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="39" style="5" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.3">

</xml_diff>